<commit_message>
highlighted best results of each dataset with spok model
</commit_message>
<xml_diff>
--- a/results_analysis/spok_covertype_ttt.xlsx
+++ b/results_analysis/spok_covertype_ttt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\matlab-mltool-fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF406CD-294E-4BC8-AAA5-5CF6B63AE7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D515CA8F-8EDB-48C2-AAEC-DBEE1ED3C2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_final" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,28 @@
     <sheet name="hp_kernel" sheetId="12" r:id="rId9"/>
     <sheet name="v1_v2" sheetId="13" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="32">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -142,7 +153,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,13 +161,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="28">
@@ -518,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -704,6 +729,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -988,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,7 +1025,7 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
@@ -1321,7 +1349,7 @@
         <v>0.87918353413377703</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1331,98 +1359,370 @@
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="50">
+        <f>1-D5</f>
+        <v>0.11856823651924397</v>
+      </c>
+      <c r="E15" s="50">
+        <f t="shared" ref="E15:K15" si="0">1-E5</f>
+        <v>0.11005289545733499</v>
+      </c>
+      <c r="F15" s="50">
+        <f t="shared" si="0"/>
+        <v>0.12224229843520495</v>
+      </c>
+      <c r="G15" s="50">
+        <f t="shared" si="0"/>
+        <v>0.11327524258118804</v>
+      </c>
+      <c r="H15" s="50">
+        <f t="shared" si="0"/>
+        <v>0.11224767763425603</v>
+      </c>
+      <c r="I15" s="50">
+        <f t="shared" si="0"/>
+        <v>0.13355758156727804</v>
+      </c>
+      <c r="J15" s="50">
+        <f t="shared" si="0"/>
+        <v>0.11603035799259298</v>
+      </c>
+      <c r="K15" s="50">
+        <f t="shared" si="0"/>
+        <v>0.11827858733957197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="50">
+        <f t="shared" ref="D16:K16" si="1">1-D6</f>
+        <v>0.11875788776783902</v>
+      </c>
+      <c r="E16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.11386833375861205</v>
+      </c>
+      <c r="F16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.11962166300007604</v>
+      </c>
+      <c r="G16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.12758529133880003</v>
+      </c>
+      <c r="H16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.12306986751998195</v>
+      </c>
+      <c r="I16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.16101391005703303</v>
+      </c>
+      <c r="J16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.11926649793452504</v>
+      </c>
+      <c r="K16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.12074577767356498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="50">
+        <f t="shared" ref="D17:K17" si="2">1-D7</f>
+        <v>0.11296662827665604</v>
+      </c>
+      <c r="E17" s="50">
+        <f t="shared" si="2"/>
+        <v>0.12818183072074396</v>
+      </c>
+      <c r="F17" s="50">
+        <f t="shared" si="2"/>
+        <v>0.11023909850141</v>
+      </c>
+      <c r="G17" s="50">
+        <f t="shared" si="2"/>
+        <v>0.11038047488672598</v>
+      </c>
+      <c r="H17" s="50">
+        <f t="shared" si="2"/>
+        <v>0.11243215657607097</v>
+      </c>
+      <c r="I17" s="50">
+        <f t="shared" si="2"/>
+        <v>0.12824045019758201</v>
+      </c>
+      <c r="J17" s="63">
+        <f t="shared" si="2"/>
+        <v>0.10624262946283902</v>
+      </c>
+      <c r="K17" s="50">
+        <f t="shared" si="2"/>
+        <v>0.11085977531499303</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="63">
+        <f t="shared" ref="D18:K18" si="3">1-D8</f>
+        <v>0.10845120445783896</v>
+      </c>
+      <c r="E18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.12296986958890499</v>
+      </c>
+      <c r="F18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.14376081874168101</v>
+      </c>
+      <c r="G18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.12470086825789795</v>
+      </c>
+      <c r="H18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.117473431584174</v>
+      </c>
+      <c r="I18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.13375240512265296</v>
+      </c>
+      <c r="J18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.18349965173134297</v>
+      </c>
+      <c r="K18" s="50">
+        <f t="shared" si="3"/>
+        <v>0.11674068812369398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="50">
+        <f t="shared" ref="D19:K19" si="4">1-D9</f>
+        <v>0.114618318241692</v>
+      </c>
+      <c r="E19" s="50">
+        <f t="shared" si="4"/>
+        <v>0.11272352985800305</v>
+      </c>
+      <c r="F19" s="50">
+        <f t="shared" si="4"/>
+        <v>0.11352523740888099</v>
+      </c>
+      <c r="G19" s="50">
+        <f t="shared" si="4"/>
+        <v>0.114618318241692</v>
+      </c>
+      <c r="H19" s="50">
+        <f t="shared" si="4"/>
+        <v>0.114618318241692</v>
+      </c>
+      <c r="I19" s="50">
+        <f t="shared" si="4"/>
+        <v>0.114618318241692</v>
+      </c>
+      <c r="J19" s="50">
+        <f t="shared" si="4"/>
+        <v>0.11075115687261605</v>
+      </c>
+      <c r="K19" s="50">
+        <f t="shared" si="4"/>
+        <v>0.114618318241692</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="50">
+        <f t="shared" ref="D20:K20" si="5">1-D10</f>
+        <v>0.13711612863182099</v>
+      </c>
+      <c r="E20" s="50">
+        <f t="shared" si="5"/>
+        <v>0.145331475900499</v>
+      </c>
+      <c r="F20" s="50">
+        <f t="shared" si="5"/>
+        <v>0.13514547974869495</v>
+      </c>
+      <c r="G20" s="50">
+        <f t="shared" si="5"/>
+        <v>0.13109556354006502</v>
+      </c>
+      <c r="H20" s="50">
+        <f t="shared" si="5"/>
+        <v>0.11884236877857701</v>
+      </c>
+      <c r="I20" s="50">
+        <f t="shared" si="5"/>
+        <v>0.12834906863995899</v>
+      </c>
+      <c r="J20" s="50">
+        <f t="shared" si="5"/>
+        <v>0.16304490251925796</v>
+      </c>
+      <c r="K20" s="50">
+        <f t="shared" si="5"/>
+        <v>0.14509354978862499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="50">
+        <f t="shared" ref="D21:K21" si="6">1-D11</f>
+        <v>0.12981800376543895</v>
+      </c>
+      <c r="E21" s="50">
+        <f t="shared" si="6"/>
+        <v>0.11368385481679699</v>
+      </c>
+      <c r="F21" s="50">
+        <f t="shared" si="6"/>
+        <v>0.12404743350137604</v>
+      </c>
+      <c r="G21" s="50">
+        <f t="shared" si="6"/>
+        <v>0.11569415805190197</v>
+      </c>
+      <c r="H21" s="50">
+        <f t="shared" si="6"/>
+        <v>0.11273904677834301</v>
+      </c>
+      <c r="I21" s="50">
+        <f t="shared" si="6"/>
+        <v>0.11957856044357695</v>
+      </c>
+      <c r="J21" s="50">
+        <f t="shared" si="6"/>
+        <v>0.16667241367420005</v>
+      </c>
+      <c r="K21" s="50">
+        <f t="shared" si="6"/>
+        <v>0.11592863595925595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="50">
+        <f t="shared" ref="D22:K22" si="7">1-D12</f>
+        <v>0.13582822424363605</v>
+      </c>
+      <c r="E22" s="50">
+        <f t="shared" si="7"/>
+        <v>0.12367330331096604</v>
+      </c>
+      <c r="F22" s="50">
+        <f t="shared" si="7"/>
+        <v>0.17550498955194005</v>
+      </c>
+      <c r="G22" s="50">
+        <f t="shared" si="7"/>
+        <v>0.12512499741384697</v>
+      </c>
+      <c r="H22" s="50">
+        <f t="shared" si="7"/>
+        <v>0.132073129521458</v>
+      </c>
+      <c r="I22" s="50">
+        <f t="shared" si="7"/>
+        <v>0.13434377219781701</v>
+      </c>
+      <c r="J22" s="50">
+        <f t="shared" si="7"/>
+        <v>0.13025937394398701</v>
+      </c>
+      <c r="K22" s="50">
+        <f t="shared" si="7"/>
+        <v>0.12081646586622297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -1432,7 +1732,7 @@
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
     </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -1442,7 +1742,7 @@
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -1452,18 +1752,16 @@
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
     </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
     </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D27" s="15"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -1472,7 +1770,7 @@
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
     </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -1482,17 +1780,17 @@
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
     </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1502,7 +1800,7 @@
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1512,7 +1810,7 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -1657,6 +1955,7 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1664,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -4835,7 +5134,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>